<commit_message>
final changes to notebooks
</commit_message>
<xml_diff>
--- a/data/working data/esg_score_all.xlsx
+++ b/data/working data/esg_score_all.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paloma/Desktop/Ironhack/proyecto_final/data/working data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paloma/Desktop/Ironhack/sustainability-esg-scoring/data/working data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DFB617-2105-394E-9387-1BED23CB65A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C39E1B8D-5092-5E45-B7FE-861B8EE179EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2233,9 +2233,6 @@
     <t>TRV</t>
   </si>
   <si>
-    <t>The Travelers Companies, Inc.</t>
-  </si>
-  <si>
     <t>TFC</t>
   </si>
   <si>
@@ -2371,9 +2368,6 @@
     <t>WMB</t>
   </si>
   <si>
-    <t>The Williams Companies, Inc.</t>
-  </si>
-  <si>
     <t>MSCI</t>
   </si>
   <si>
@@ -4142,6 +4136,12 @@
   </si>
   <si>
     <t>American Water Works Co., Inc.</t>
+  </si>
+  <si>
+    <t>The Travelers Cos., Inc.</t>
+  </si>
+  <si>
+    <t>The Williams Cos., Inc.</t>
   </si>
 </sst>
 </file>
@@ -4507,8 +4507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E613"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117:XFD117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6301,7 +6301,7 @@
         <v>234</v>
       </c>
       <c r="B117" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="C117" t="s">
         <v>235</v>
@@ -6318,7 +6318,7 @@
         <v>238</v>
       </c>
       <c r="B118" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="C118" t="s">
         <v>239</v>
@@ -6335,7 +6335,7 @@
         <v>242</v>
       </c>
       <c r="B119" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="C119" t="s">
         <v>243</v>
@@ -6420,7 +6420,7 @@
         <v>264</v>
       </c>
       <c r="B124" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C124" t="s">
         <v>263</v>
@@ -6437,7 +6437,7 @@
         <v>265</v>
       </c>
       <c r="B125" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="C125" t="s">
         <v>266</v>
@@ -6488,7 +6488,7 @@
         <v>274</v>
       </c>
       <c r="B128" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="C128" t="s">
         <v>275</v>
@@ -6539,7 +6539,7 @@
         <v>288</v>
       </c>
       <c r="B131" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="C131" t="s">
         <v>289</v>
@@ -6556,7 +6556,7 @@
         <v>292</v>
       </c>
       <c r="B132" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="C132" t="s">
         <v>293</v>
@@ -6573,7 +6573,7 @@
         <v>296</v>
       </c>
       <c r="B133" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="C133" t="s">
         <v>297</v>
@@ -6590,7 +6590,7 @@
         <v>299</v>
       </c>
       <c r="B134" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C134" t="s">
         <v>300</v>
@@ -6641,7 +6641,7 @@
         <v>308</v>
       </c>
       <c r="B137" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="C137" t="s">
         <v>309</v>
@@ -6692,7 +6692,7 @@
         <v>316</v>
       </c>
       <c r="B140" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="C140" t="s">
         <v>263</v>
@@ -6709,7 +6709,7 @@
         <v>317</v>
       </c>
       <c r="B141" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C141" t="s">
         <v>318</v>
@@ -6726,7 +6726,7 @@
         <v>319</v>
       </c>
       <c r="B142" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="C142" t="s">
         <v>320</v>
@@ -6760,7 +6760,7 @@
         <v>328</v>
       </c>
       <c r="B144" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C144" t="s">
         <v>239</v>
@@ -6794,7 +6794,7 @@
         <v>333</v>
       </c>
       <c r="B146" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="C146" t="s">
         <v>334</v>
@@ -6811,7 +6811,7 @@
         <v>336</v>
       </c>
       <c r="B147" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="C147" t="s">
         <v>337</v>
@@ -6845,7 +6845,7 @@
         <v>342</v>
       </c>
       <c r="B149" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="C149" t="s">
         <v>343</v>
@@ -6862,7 +6862,7 @@
         <v>345</v>
       </c>
       <c r="B150" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="C150" t="s">
         <v>325</v>
@@ -6879,7 +6879,7 @@
         <v>15</v>
       </c>
       <c r="B151" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="C151" t="s">
         <v>347</v>
@@ -6896,7 +6896,7 @@
         <v>350</v>
       </c>
       <c r="B152" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="C152" t="s">
         <v>351</v>
@@ -6947,7 +6947,7 @@
         <v>355</v>
       </c>
       <c r="B155" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="C155" t="s">
         <v>263</v>
@@ -6981,7 +6981,7 @@
         <v>358</v>
       </c>
       <c r="B157" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="C157" t="s">
         <v>359</v>
@@ -7015,7 +7015,7 @@
         <v>364</v>
       </c>
       <c r="B159" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="C159" t="s">
         <v>263</v>
@@ -7032,7 +7032,7 @@
         <v>365</v>
       </c>
       <c r="B160" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="C160" t="s">
         <v>263</v>
@@ -7066,7 +7066,7 @@
         <v>368</v>
       </c>
       <c r="B162" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="C162" t="s">
         <v>331</v>
@@ -7083,7 +7083,7 @@
         <v>371</v>
       </c>
       <c r="B163" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="C163" t="s">
         <v>293</v>
@@ -7134,7 +7134,7 @@
         <v>380</v>
       </c>
       <c r="B166" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C166" t="s">
         <v>381</v>
@@ -7151,7 +7151,7 @@
         <v>383</v>
       </c>
       <c r="B167" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="C167" t="s">
         <v>351</v>
@@ -7168,7 +7168,7 @@
         <v>384</v>
       </c>
       <c r="B168" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C168" t="s">
         <v>244</v>
@@ -7185,7 +7185,7 @@
         <v>385</v>
       </c>
       <c r="B169" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="C169" t="s">
         <v>263</v>
@@ -7202,7 +7202,7 @@
         <v>386</v>
       </c>
       <c r="B170" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="C170" t="s">
         <v>363</v>
@@ -7219,7 +7219,7 @@
         <v>388</v>
       </c>
       <c r="B171" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="C171" t="s">
         <v>389</v>
@@ -7236,7 +7236,7 @@
         <v>392</v>
       </c>
       <c r="B172" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="C172" t="s">
         <v>275</v>
@@ -7270,7 +7270,7 @@
         <v>397</v>
       </c>
       <c r="B174" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="C174" t="s">
         <v>322</v>
@@ -7287,7 +7287,7 @@
         <v>400</v>
       </c>
       <c r="B175" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C175" t="s">
         <v>401</v>
@@ -7304,7 +7304,7 @@
         <v>402</v>
       </c>
       <c r="B176" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C176" t="s">
         <v>403</v>
@@ -7338,7 +7338,7 @@
         <v>406</v>
       </c>
       <c r="B178" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="C178" t="s">
         <v>340</v>
@@ -7355,7 +7355,7 @@
         <v>407</v>
       </c>
       <c r="B179" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="C179" t="s">
         <v>282</v>
@@ -7423,7 +7423,7 @@
         <v>414</v>
       </c>
       <c r="B183" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="C183" t="s">
         <v>271</v>
@@ -7440,7 +7440,7 @@
         <v>415</v>
       </c>
       <c r="B184" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="C184" t="s">
         <v>266</v>
@@ -7474,7 +7474,7 @@
         <v>419</v>
       </c>
       <c r="B186" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="C186" t="s">
         <v>263</v>
@@ -7491,7 +7491,7 @@
         <v>420</v>
       </c>
       <c r="B187" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="C187" t="s">
         <v>421</v>
@@ -7508,7 +7508,7 @@
         <v>423</v>
       </c>
       <c r="B188" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="C188" t="s">
         <v>263</v>
@@ -7525,7 +7525,7 @@
         <v>424</v>
       </c>
       <c r="B189" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="C189" t="s">
         <v>425</v>
@@ -7576,7 +7576,7 @@
         <v>431</v>
       </c>
       <c r="B192" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="C192" t="s">
         <v>263</v>
@@ -7644,7 +7644,7 @@
         <v>440</v>
       </c>
       <c r="B196" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C196" t="s">
         <v>401</v>
@@ -7661,7 +7661,7 @@
         <v>443</v>
       </c>
       <c r="B197" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="C197" t="s">
         <v>293</v>
@@ -7712,7 +7712,7 @@
         <v>451</v>
       </c>
       <c r="B200" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="C200" t="s">
         <v>442</v>
@@ -7780,7 +7780,7 @@
         <v>462</v>
       </c>
       <c r="B204" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="C204" t="s">
         <v>382</v>
@@ -7814,7 +7814,7 @@
         <v>466</v>
       </c>
       <c r="B206" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="C206" t="s">
         <v>263</v>
@@ -7848,7 +7848,7 @@
         <v>468</v>
       </c>
       <c r="B208" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="C208" t="s">
         <v>280</v>
@@ -7865,7 +7865,7 @@
         <v>470</v>
       </c>
       <c r="B209" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C209" t="s">
         <v>320</v>
@@ -7882,7 +7882,7 @@
         <v>472</v>
       </c>
       <c r="B210" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="C210" t="s">
         <v>473</v>
@@ -7899,7 +7899,7 @@
         <v>475</v>
       </c>
       <c r="B211" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="C211" t="s">
         <v>263</v>
@@ -7933,7 +7933,7 @@
         <v>476</v>
       </c>
       <c r="B213" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="C213" t="s">
         <v>389</v>
@@ -7950,7 +7950,7 @@
         <v>38</v>
       </c>
       <c r="B214" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="C214" t="s">
         <v>450</v>
@@ -7984,7 +7984,7 @@
         <v>481</v>
       </c>
       <c r="B216" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="C216" t="s">
         <v>340</v>
@@ -8001,7 +8001,7 @@
         <v>482</v>
       </c>
       <c r="B217" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="C217" t="s">
         <v>235</v>
@@ -8035,7 +8035,7 @@
         <v>484</v>
       </c>
       <c r="B219" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="C219" t="s">
         <v>275</v>
@@ -8069,7 +8069,7 @@
         <v>491</v>
       </c>
       <c r="B221" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="C221" t="s">
         <v>492</v>
@@ -8103,7 +8103,7 @@
         <v>496</v>
       </c>
       <c r="B223" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="C223" t="s">
         <v>263</v>
@@ -8137,7 +8137,7 @@
         <v>499</v>
       </c>
       <c r="B225" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="C225" t="s">
         <v>263</v>
@@ -8154,7 +8154,7 @@
         <v>500</v>
       </c>
       <c r="B226" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="C226" t="s">
         <v>347</v>
@@ -8205,7 +8205,7 @@
         <v>506</v>
       </c>
       <c r="B229" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="C229" t="s">
         <v>307</v>
@@ -8222,7 +8222,7 @@
         <v>507</v>
       </c>
       <c r="B230" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="C230" t="s">
         <v>258</v>
@@ -8239,7 +8239,7 @@
         <v>509</v>
       </c>
       <c r="B231" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="C231" t="s">
         <v>360</v>
@@ -8273,7 +8273,7 @@
         <v>514</v>
       </c>
       <c r="B233" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="C233" t="s">
         <v>263</v>
@@ -8290,7 +8290,7 @@
         <v>515</v>
       </c>
       <c r="B234" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="C234" t="s">
         <v>235</v>
@@ -8324,7 +8324,7 @@
         <v>518</v>
       </c>
       <c r="B236" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="C236" t="s">
         <v>293</v>
@@ -8375,7 +8375,7 @@
         <v>526</v>
       </c>
       <c r="B239" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="C239" t="s">
         <v>320</v>
@@ -8392,7 +8392,7 @@
         <v>527</v>
       </c>
       <c r="B240" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="C240" t="s">
         <v>263</v>
@@ -8443,7 +8443,7 @@
         <v>533</v>
       </c>
       <c r="B243" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="C243" t="s">
         <v>534</v>
@@ -8460,7 +8460,7 @@
         <v>535</v>
       </c>
       <c r="B244" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="C244" t="s">
         <v>240</v>
@@ -8477,7 +8477,7 @@
         <v>536</v>
       </c>
       <c r="B245" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="C245" t="s">
         <v>293</v>
@@ -8511,7 +8511,7 @@
         <v>541</v>
       </c>
       <c r="B247" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="C247" t="s">
         <v>263</v>
@@ -8562,7 +8562,7 @@
         <v>548</v>
       </c>
       <c r="B250" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="C250" t="s">
         <v>263</v>
@@ -8579,7 +8579,7 @@
         <v>549</v>
       </c>
       <c r="B251" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="C251" t="s">
         <v>263</v>
@@ -8613,7 +8613,7 @@
         <v>552</v>
       </c>
       <c r="B253" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="C253" t="s">
         <v>540</v>
@@ -8698,7 +8698,7 @@
         <v>562</v>
       </c>
       <c r="B258" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="C258" t="s">
         <v>393</v>
@@ -8732,7 +8732,7 @@
         <v>565</v>
       </c>
       <c r="B260" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="C260" t="s">
         <v>437</v>
@@ -8749,7 +8749,7 @@
         <v>566</v>
       </c>
       <c r="B261" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="C261" t="s">
         <v>263</v>
@@ -8766,7 +8766,7 @@
         <v>567</v>
       </c>
       <c r="B262" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="C262" t="s">
         <v>244</v>
@@ -8800,7 +8800,7 @@
         <v>569</v>
       </c>
       <c r="B264" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="C264" t="s">
         <v>263</v>
@@ -8817,7 +8817,7 @@
         <v>570</v>
       </c>
       <c r="B265" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="C265" t="s">
         <v>421</v>
@@ -8851,7 +8851,7 @@
         <v>574</v>
       </c>
       <c r="B267" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="C267" t="s">
         <v>263</v>
@@ -8885,7 +8885,7 @@
         <v>577</v>
       </c>
       <c r="B269" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="C269" t="s">
         <v>325</v>
@@ -8919,7 +8919,7 @@
         <v>580</v>
       </c>
       <c r="B271" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="C271" t="s">
         <v>452</v>
@@ -8936,7 +8936,7 @@
         <v>581</v>
       </c>
       <c r="B272" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="C272" t="s">
         <v>263</v>
@@ -8970,7 +8970,7 @@
         <v>584</v>
       </c>
       <c r="B274" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="C274" t="s">
         <v>585</v>
@@ -9004,7 +9004,7 @@
         <v>588</v>
       </c>
       <c r="B276" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="C276" t="s">
         <v>412</v>
@@ -9021,7 +9021,7 @@
         <v>589</v>
       </c>
       <c r="B277" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="C277" t="s">
         <v>477</v>
@@ -9055,7 +9055,7 @@
         <v>592</v>
       </c>
       <c r="B279" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="C279" t="s">
         <v>522</v>
@@ -9072,7 +9072,7 @@
         <v>593</v>
       </c>
       <c r="B280" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C280" t="s">
         <v>452</v>
@@ -9089,7 +9089,7 @@
         <v>594</v>
       </c>
       <c r="B281" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="C281" t="s">
         <v>241</v>
@@ -9140,7 +9140,7 @@
         <v>600</v>
       </c>
       <c r="B284" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="C284" t="s">
         <v>255</v>
@@ -9157,7 +9157,7 @@
         <v>601</v>
       </c>
       <c r="B285" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="C285" t="s">
         <v>298</v>
@@ -9191,7 +9191,7 @@
         <v>605</v>
       </c>
       <c r="B287" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="C287" t="s">
         <v>399</v>
@@ -9208,7 +9208,7 @@
         <v>606</v>
       </c>
       <c r="B288" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="C288" t="s">
         <v>293</v>
@@ -9225,7 +9225,7 @@
         <v>607</v>
       </c>
       <c r="B289" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="C289" t="s">
         <v>253</v>
@@ -9259,7 +9259,7 @@
         <v>610</v>
       </c>
       <c r="B291" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="C291" t="s">
         <v>396</v>
@@ -9276,7 +9276,7 @@
         <v>611</v>
       </c>
       <c r="B292" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C292" t="s">
         <v>253</v>
@@ -9293,7 +9293,7 @@
         <v>612</v>
       </c>
       <c r="B293" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C293" t="s">
         <v>344</v>
@@ -9310,7 +9310,7 @@
         <v>613</v>
       </c>
       <c r="B294" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C294" t="s">
         <v>282</v>
@@ -9412,7 +9412,7 @@
         <v>625</v>
       </c>
       <c r="B300" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="C300" t="s">
         <v>263</v>
@@ -9429,7 +9429,7 @@
         <v>626</v>
       </c>
       <c r="B301" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="C301" t="s">
         <v>413</v>
@@ -9446,7 +9446,7 @@
         <v>627</v>
       </c>
       <c r="B302" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="C302" t="s">
         <v>263</v>
@@ -9463,7 +9463,7 @@
         <v>628</v>
       </c>
       <c r="B303" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="C303" t="s">
         <v>271</v>
@@ -9480,7 +9480,7 @@
         <v>629</v>
       </c>
       <c r="B304" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C304" t="s">
         <v>347</v>
@@ -9514,7 +9514,7 @@
         <v>633</v>
       </c>
       <c r="B306" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="C306" t="s">
         <v>634</v>
@@ -9531,7 +9531,7 @@
         <v>635</v>
       </c>
       <c r="B307" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="C307" t="s">
         <v>636</v>
@@ -9548,7 +9548,7 @@
         <v>84</v>
       </c>
       <c r="B308" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="C308" t="s">
         <v>349</v>
@@ -9616,7 +9616,7 @@
         <v>643</v>
       </c>
       <c r="B312" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="C312" t="s">
         <v>302</v>
@@ -9650,7 +9650,7 @@
         <v>646</v>
       </c>
       <c r="B314" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="C314" t="s">
         <v>396</v>
@@ -9718,7 +9718,7 @@
         <v>652</v>
       </c>
       <c r="B318" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="C318" t="s">
         <v>263</v>
@@ -9752,7 +9752,7 @@
         <v>655</v>
       </c>
       <c r="B320" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="C320" t="s">
         <v>656</v>
@@ -9769,7 +9769,7 @@
         <v>657</v>
       </c>
       <c r="B321" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="C321" t="s">
         <v>478</v>
@@ -9837,7 +9837,7 @@
         <v>664</v>
       </c>
       <c r="B325" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="C325" t="s">
         <v>571</v>
@@ -9888,7 +9888,7 @@
         <v>670</v>
       </c>
       <c r="B328" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="C328" t="s">
         <v>307</v>
@@ -9922,7 +9922,7 @@
         <v>673</v>
       </c>
       <c r="B330" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="C330" t="s">
         <v>253</v>
@@ -9973,7 +9973,7 @@
         <v>679</v>
       </c>
       <c r="B333" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="C333" t="s">
         <v>263</v>
@@ -9990,7 +9990,7 @@
         <v>680</v>
       </c>
       <c r="B334" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="C334" t="s">
         <v>263</v>
@@ -10007,7 +10007,7 @@
         <v>98</v>
       </c>
       <c r="B335" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="C335" t="s">
         <v>263</v>
@@ -10024,7 +10024,7 @@
         <v>681</v>
       </c>
       <c r="B336" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="C336" t="s">
         <v>682</v>
@@ -10041,7 +10041,7 @@
         <v>683</v>
       </c>
       <c r="B337" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="C337" t="s">
         <v>286</v>
@@ -10092,7 +10092,7 @@
         <v>688</v>
       </c>
       <c r="B340" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="C340" t="s">
         <v>534</v>
@@ -10160,7 +10160,7 @@
         <v>695</v>
       </c>
       <c r="B344" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="C344" t="s">
         <v>263</v>
@@ -10177,7 +10177,7 @@
         <v>696</v>
       </c>
       <c r="B345" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C345" t="s">
         <v>263</v>
@@ -10228,7 +10228,7 @@
         <v>701</v>
       </c>
       <c r="B348" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="C348" t="s">
         <v>375</v>
@@ -10245,7 +10245,7 @@
         <v>703</v>
       </c>
       <c r="B349" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C349" t="s">
         <v>704</v>
@@ -10262,7 +10262,7 @@
         <v>705</v>
       </c>
       <c r="B350" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="C350" t="s">
         <v>263</v>
@@ -10347,7 +10347,7 @@
         <v>714</v>
       </c>
       <c r="B355" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="C355" t="s">
         <v>378</v>
@@ -10364,7 +10364,7 @@
         <v>716</v>
       </c>
       <c r="B356" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="C356" t="s">
         <v>263</v>
@@ -10381,7 +10381,7 @@
         <v>717</v>
       </c>
       <c r="B357" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="C357" t="s">
         <v>340</v>
@@ -10415,7 +10415,7 @@
         <v>720</v>
       </c>
       <c r="B359" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="C359" t="s">
         <v>321</v>
@@ -10432,7 +10432,7 @@
         <v>721</v>
       </c>
       <c r="B360" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="C360" t="s">
         <v>237</v>
@@ -10466,7 +10466,7 @@
         <v>106</v>
       </c>
       <c r="B362" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="C362" t="s">
         <v>263</v>
@@ -10483,7 +10483,7 @@
         <v>108</v>
       </c>
       <c r="B363" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="C363" t="s">
         <v>263</v>
@@ -10517,7 +10517,7 @@
         <v>727</v>
       </c>
       <c r="B365" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="C365" t="s">
         <v>263</v>
@@ -10585,7 +10585,7 @@
         <v>734</v>
       </c>
       <c r="B369" t="s">
-        <v>735</v>
+        <v>1370</v>
       </c>
       <c r="C369" t="s">
         <v>389</v>
@@ -10599,10 +10599,10 @@
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B370" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="C370" t="s">
         <v>263</v>
@@ -10616,13 +10616,13 @@
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
+        <v>736</v>
+      </c>
+      <c r="B371" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C371" t="s">
         <v>737</v>
-      </c>
-      <c r="B371" t="s">
-        <v>1153</v>
-      </c>
-      <c r="C371" t="s">
-        <v>738</v>
       </c>
       <c r="D371" t="s">
         <v>240</v>
@@ -10633,10 +10633,10 @@
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
+        <v>738</v>
+      </c>
+      <c r="B372" t="s">
         <v>739</v>
-      </c>
-      <c r="B372" t="s">
-        <v>740</v>
       </c>
       <c r="C372" t="s">
         <v>285</v>
@@ -10650,10 +10650,10 @@
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
+        <v>740</v>
+      </c>
+      <c r="B373" t="s">
         <v>741</v>
-      </c>
-      <c r="B373" t="s">
-        <v>742</v>
       </c>
       <c r="C373" t="s">
         <v>275</v>
@@ -10667,10 +10667,10 @@
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B374" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="C374" t="s">
         <v>546</v>
@@ -10687,7 +10687,7 @@
         <v>114</v>
       </c>
       <c r="B375" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C375" t="s">
         <v>263</v>
@@ -10701,10 +10701,10 @@
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B376" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="C376" t="s">
         <v>240</v>
@@ -10718,10 +10718,10 @@
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B377" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="C377" t="s">
         <v>682</v>
@@ -10735,10 +10735,10 @@
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
+        <v>746</v>
+      </c>
+      <c r="B378" t="s">
         <v>747</v>
-      </c>
-      <c r="B378" t="s">
-        <v>748</v>
       </c>
       <c r="C378" t="s">
         <v>382</v>
@@ -10752,10 +10752,10 @@
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
+        <v>748</v>
+      </c>
+      <c r="B379" t="s">
         <v>749</v>
-      </c>
-      <c r="B379" t="s">
-        <v>750</v>
       </c>
       <c r="C379" t="s">
         <v>525</v>
@@ -10769,10 +10769,10 @@
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B380" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="C380" t="s">
         <v>503</v>
@@ -10786,10 +10786,10 @@
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
+        <v>751</v>
+      </c>
+      <c r="B381" t="s">
         <v>752</v>
-      </c>
-      <c r="B381" t="s">
-        <v>753</v>
       </c>
       <c r="C381" t="s">
         <v>241</v>
@@ -10803,10 +10803,10 @@
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B382" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="C382" t="s">
         <v>492</v>
@@ -10820,10 +10820,10 @@
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
+        <v>754</v>
+      </c>
+      <c r="B383" t="s">
         <v>755</v>
-      </c>
-      <c r="B383" t="s">
-        <v>756</v>
       </c>
       <c r="C383" t="s">
         <v>724</v>
@@ -10837,10 +10837,10 @@
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
+        <v>756</v>
+      </c>
+      <c r="B384" t="s">
         <v>757</v>
-      </c>
-      <c r="B384" t="s">
-        <v>758</v>
       </c>
       <c r="C384" t="s">
         <v>325</v>
@@ -10854,10 +10854,10 @@
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
+        <v>758</v>
+      </c>
+      <c r="B385" t="s">
         <v>759</v>
-      </c>
-      <c r="B385" t="s">
-        <v>760</v>
       </c>
       <c r="C385" t="s">
         <v>263</v>
@@ -10871,10 +10871,10 @@
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B386" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="C386" t="s">
         <v>263</v>
@@ -10888,13 +10888,13 @@
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
+        <v>761</v>
+      </c>
+      <c r="B387" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C387" t="s">
         <v>762</v>
-      </c>
-      <c r="B387" t="s">
-        <v>1285</v>
-      </c>
-      <c r="C387" t="s">
-        <v>763</v>
       </c>
       <c r="D387" t="s">
         <v>255</v>
@@ -10905,10 +10905,10 @@
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B388" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="C388" t="s">
         <v>349</v>
@@ -10922,10 +10922,10 @@
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
+        <v>764</v>
+      </c>
+      <c r="B389" t="s">
         <v>765</v>
-      </c>
-      <c r="B389" t="s">
-        <v>766</v>
       </c>
       <c r="C389" t="s">
         <v>381</v>
@@ -10939,10 +10939,10 @@
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B390" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="C390" t="s">
         <v>416</v>
@@ -10956,10 +10956,10 @@
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
+        <v>767</v>
+      </c>
+      <c r="B391" t="s">
         <v>768</v>
-      </c>
-      <c r="B391" t="s">
-        <v>769</v>
       </c>
       <c r="C391" t="s">
         <v>508</v>
@@ -10973,10 +10973,10 @@
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
+        <v>769</v>
+      </c>
+      <c r="B392" t="s">
         <v>770</v>
-      </c>
-      <c r="B392" t="s">
-        <v>771</v>
       </c>
       <c r="C392" t="s">
         <v>263</v>
@@ -10990,10 +10990,10 @@
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
+        <v>771</v>
+      </c>
+      <c r="B393" t="s">
         <v>772</v>
-      </c>
-      <c r="B393" t="s">
-        <v>773</v>
       </c>
       <c r="C393" t="s">
         <v>387</v>
@@ -11007,10 +11007,10 @@
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B394" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="C394" t="s">
         <v>530</v>
@@ -11024,13 +11024,13 @@
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
+        <v>774</v>
+      </c>
+      <c r="B395" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C395" t="s">
         <v>775</v>
-      </c>
-      <c r="B395" t="s">
-        <v>1286</v>
-      </c>
-      <c r="C395" t="s">
-        <v>776</v>
       </c>
       <c r="D395" t="s">
         <v>277</v>
@@ -11041,10 +11041,10 @@
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B396" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="C396" t="s">
         <v>595</v>
@@ -11058,13 +11058,13 @@
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
+        <v>777</v>
+      </c>
+      <c r="B397" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C397" t="s">
         <v>778</v>
-      </c>
-      <c r="B397" t="s">
-        <v>1370</v>
-      </c>
-      <c r="C397" t="s">
-        <v>779</v>
       </c>
       <c r="D397" t="s">
         <v>399</v>
@@ -11075,10 +11075,10 @@
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B398" t="s">
-        <v>781</v>
+        <v>1371</v>
       </c>
       <c r="C398" t="s">
         <v>547</v>
@@ -11092,10 +11092,10 @@
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="B399" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="C399" t="s">
         <v>253</v>
@@ -11109,10 +11109,10 @@
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B400" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="C400" t="s">
         <v>263</v>
@@ -11126,10 +11126,10 @@
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B401" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C401" t="s">
         <v>437</v>
@@ -11143,10 +11143,10 @@
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B402" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="C402" t="s">
         <v>360</v>
@@ -11160,10 +11160,10 @@
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="B403" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C403" t="s">
         <v>285</v>
@@ -11177,10 +11177,10 @@
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B404" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="C404" t="s">
         <v>530</v>
@@ -11194,10 +11194,10 @@
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B405" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="C405" t="s">
         <v>309</v>
@@ -11211,10 +11211,10 @@
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B406" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="C406" t="s">
         <v>263</v>
@@ -11228,10 +11228,10 @@
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B407" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="C407" t="s">
         <v>305</v>
@@ -11245,10 +11245,10 @@
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B408" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="C408" t="s">
         <v>442</v>
@@ -11262,10 +11262,10 @@
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B409" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="C409" t="s">
         <v>263</v>
@@ -11279,10 +11279,10 @@
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B410" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="C410" t="s">
         <v>263</v>
@@ -11296,10 +11296,10 @@
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="B411" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="C411" t="s">
         <v>322</v>
@@ -11313,10 +11313,10 @@
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B412" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="C412" t="s">
         <v>422</v>
@@ -11347,10 +11347,10 @@
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B414" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="C414" t="s">
         <v>604</v>
@@ -11364,10 +11364,10 @@
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B415" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="C415" t="s">
         <v>322</v>
@@ -11381,10 +11381,10 @@
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="B416" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C416" t="s">
         <v>340</v>
@@ -11398,10 +11398,10 @@
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B417" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="C417" t="s">
         <v>263</v>
@@ -11415,10 +11415,10 @@
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B418" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="C418" t="s">
         <v>285</v>
@@ -11432,10 +11432,10 @@
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B419" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C419" t="s">
         <v>412</v>
@@ -11449,10 +11449,10 @@
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B420" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="C420" t="s">
         <v>389</v>
@@ -11466,10 +11466,10 @@
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B421" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="C421" t="s">
         <v>237</v>
@@ -11478,21 +11478,21 @@
         <v>390</v>
       </c>
       <c r="E421" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B422" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="C422" t="s">
         <v>293</v>
       </c>
       <c r="D422" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="E422" t="s">
         <v>478</v>
@@ -11500,10 +11500,10 @@
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B423" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="C423" t="s">
         <v>263</v>
@@ -11517,10 +11517,10 @@
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="B424" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C424" t="s">
         <v>263</v>
@@ -11534,10 +11534,10 @@
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="B425" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="C425" t="s">
         <v>263</v>
@@ -11551,10 +11551,10 @@
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B426" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="C426" t="s">
         <v>263</v>
@@ -11568,10 +11568,10 @@
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B427" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="C427" t="s">
         <v>263</v>
@@ -11585,10 +11585,10 @@
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B428" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C428" t="s">
         <v>272</v>
@@ -11602,10 +11602,10 @@
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="B429" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="C429" t="s">
         <v>263</v>
@@ -11619,10 +11619,10 @@
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="B430" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="C430" t="s">
         <v>471</v>
@@ -11636,10 +11636,10 @@
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="B431" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C431" t="s">
         <v>546</v>
@@ -11653,10 +11653,10 @@
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B432" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="C432" t="s">
         <v>332</v>
@@ -11670,10 +11670,10 @@
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B433" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="C433" t="s">
         <v>263</v>
@@ -11687,13 +11687,13 @@
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
+        <v>830</v>
+      </c>
+      <c r="B434" t="s">
+        <v>831</v>
+      </c>
+      <c r="C434" t="s">
         <v>832</v>
-      </c>
-      <c r="B434" t="s">
-        <v>833</v>
-      </c>
-      <c r="C434" t="s">
-        <v>834</v>
       </c>
       <c r="D434" t="s">
         <v>301</v>
@@ -11704,10 +11704,10 @@
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="B435" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C435" t="s">
         <v>263</v>
@@ -11721,10 +11721,10 @@
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="B436" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="C436" t="s">
         <v>263</v>
@@ -11738,10 +11738,10 @@
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B437" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="C437" t="s">
         <v>430</v>
@@ -11755,10 +11755,10 @@
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="B438" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="C438" t="s">
         <v>263</v>
@@ -11772,10 +11772,10 @@
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B439" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="C439" t="s">
         <v>298</v>
@@ -11789,10 +11789,10 @@
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B440" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="C440" t="s">
         <v>263</v>
@@ -11806,10 +11806,10 @@
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="B441" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="C441" t="s">
         <v>263</v>
@@ -11823,16 +11823,16 @@
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="B442" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="C442" t="s">
         <v>382</v>
       </c>
       <c r="D442" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="E442" t="s">
         <v>546</v>
@@ -11840,10 +11840,10 @@
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B443" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="C443" t="s">
         <v>291</v>
@@ -11857,10 +11857,10 @@
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="B444" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="C444" t="s">
         <v>263</v>
@@ -11874,10 +11874,10 @@
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="B445" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="C445" t="s">
         <v>243</v>
@@ -11891,10 +11891,10 @@
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="B446" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="C446" t="s">
         <v>253</v>
@@ -11908,7 +11908,7 @@
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="B447" t="s">
         <v>151</v>
@@ -11925,10 +11925,10 @@
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B448" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C448" t="s">
         <v>263</v>
@@ -11942,10 +11942,10 @@
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B449" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="C449" t="s">
         <v>263</v>
@@ -11959,10 +11959,10 @@
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B450" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="C450" t="s">
         <v>285</v>
@@ -11976,10 +11976,10 @@
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B451" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="C451" t="s">
         <v>295</v>
@@ -11993,10 +11993,10 @@
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B452" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="C452" t="s">
         <v>263</v>
@@ -12010,10 +12010,10 @@
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B453" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="C453" t="s">
         <v>263</v>
@@ -12027,10 +12027,10 @@
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="B454" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="C454" t="s">
         <v>298</v>
@@ -12044,10 +12044,10 @@
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="B455" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="C455" t="s">
         <v>240</v>
@@ -12061,13 +12061,13 @@
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B456" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C456" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D456" t="s">
         <v>490</v>
@@ -12078,10 +12078,10 @@
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B457" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="C457" t="s">
         <v>263</v>
@@ -12098,7 +12098,7 @@
         <v>154</v>
       </c>
       <c r="B458" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="C458" t="s">
         <v>263</v>
@@ -12112,10 +12112,10 @@
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="B459" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="C459" t="s">
         <v>416</v>
@@ -12129,10 +12129,10 @@
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B460" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C460" t="s">
         <v>340</v>
@@ -12146,10 +12146,10 @@
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="B461" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="C461" t="s">
         <v>340</v>
@@ -12163,10 +12163,10 @@
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="B462" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="C462" t="s">
         <v>343</v>
@@ -12180,10 +12180,10 @@
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B463" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="C463" t="s">
         <v>263</v>
@@ -12197,16 +12197,16 @@
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B464" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="C464" t="s">
         <v>656</v>
       </c>
       <c r="D464" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="E464" t="s">
         <v>341</v>
@@ -12214,10 +12214,10 @@
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B465" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="C465" t="s">
         <v>379</v>
@@ -12231,10 +12231,10 @@
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="B466" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="C466" t="s">
         <v>244</v>
@@ -12248,10 +12248,10 @@
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B467" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="C467" t="s">
         <v>715</v>
@@ -12265,10 +12265,10 @@
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="B468" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="C468" t="s">
         <v>293</v>
@@ -12282,13 +12282,13 @@
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B469" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="C469" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="D469" t="s">
         <v>291</v>
@@ -12299,10 +12299,10 @@
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="B470" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="C470" t="s">
         <v>266</v>
@@ -12316,10 +12316,10 @@
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="B471" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="C471" t="s">
         <v>263</v>
@@ -12333,10 +12333,10 @@
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B472" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C472" t="s">
         <v>340</v>
@@ -12350,10 +12350,10 @@
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="B473" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="C473" t="s">
         <v>332</v>
@@ -12367,10 +12367,10 @@
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="B474" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="C474" t="s">
         <v>458</v>
@@ -12384,16 +12384,16 @@
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="B475" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="C475" t="s">
         <v>340</v>
       </c>
       <c r="D475" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E475" t="s">
         <v>444</v>
@@ -12401,10 +12401,10 @@
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B476" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="C476" t="s">
         <v>403</v>
@@ -12418,16 +12418,16 @@
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="B477" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="C477" t="s">
         <v>425</v>
       </c>
       <c r="D477" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E477" t="s">
         <v>346</v>
@@ -12435,10 +12435,10 @@
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="B478" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="C478" t="s">
         <v>266</v>
@@ -12452,10 +12452,10 @@
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A479" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B479" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="C479" t="s">
         <v>442</v>
@@ -12469,13 +12469,13 @@
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A480" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="B480" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="C480" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="D480" t="s">
         <v>309</v>
@@ -12486,10 +12486,10 @@
     </row>
     <row r="481" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A481" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="B481" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C481" t="s">
         <v>263</v>
@@ -12503,10 +12503,10 @@
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B482" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="C482" t="s">
         <v>378</v>
@@ -12520,10 +12520,10 @@
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="B483" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C483" t="s">
         <v>263</v>
@@ -12537,10 +12537,10 @@
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="B484" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="C484" t="s">
         <v>263</v>
@@ -12554,10 +12554,10 @@
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="B485" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C485" t="s">
         <v>235</v>
@@ -12571,10 +12571,10 @@
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="B486" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C486" t="s">
         <v>399</v>
@@ -12588,10 +12588,10 @@
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B487" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="C487" t="s">
         <v>263</v>
@@ -12605,10 +12605,10 @@
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A488" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="B488" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="C488" t="s">
         <v>263</v>
@@ -12622,16 +12622,16 @@
     </row>
     <row r="489" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B489" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="C489" t="s">
         <v>374</v>
       </c>
       <c r="D489" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="E489" t="s">
         <v>240</v>
@@ -12639,10 +12639,10 @@
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="B490" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="C490" t="s">
         <v>263</v>
@@ -12656,10 +12656,10 @@
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="B491" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="C491" t="s">
         <v>263</v>
@@ -12690,10 +12690,10 @@
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B493" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="C493" t="s">
         <v>239</v>
@@ -12707,13 +12707,13 @@
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A494" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="B494" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="C494" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D494" t="s">
         <v>327</v>
@@ -12724,10 +12724,10 @@
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A495" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="B495" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C495" t="s">
         <v>280</v>
@@ -12741,10 +12741,10 @@
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A496" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="B496" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C496" t="s">
         <v>422</v>
@@ -12758,10 +12758,10 @@
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A497" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="B497" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C497" t="s">
         <v>521</v>
@@ -12775,10 +12775,10 @@
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="B498" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="C498" t="s">
         <v>375</v>
@@ -12809,10 +12809,10 @@
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="B500" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="C500" t="s">
         <v>263</v>
@@ -12826,10 +12826,10 @@
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="B501" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="C501" t="s">
         <v>511</v>
@@ -12843,10 +12843,10 @@
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B502" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="C502" t="s">
         <v>263</v>
@@ -12860,10 +12860,10 @@
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A503" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="B503" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="C503" t="s">
         <v>340</v>
@@ -12877,10 +12877,10 @@
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="B504" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="C504" t="s">
         <v>263</v>
@@ -12894,10 +12894,10 @@
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="B505" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="C505" t="s">
         <v>340</v>
@@ -12911,16 +12911,16 @@
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
+        <v>938</v>
+      </c>
+      <c r="B506" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C506" t="s">
+        <v>939</v>
+      </c>
+      <c r="D506" t="s">
         <v>940</v>
-      </c>
-      <c r="B506" t="s">
-        <v>1175</v>
-      </c>
-      <c r="C506" t="s">
-        <v>941</v>
-      </c>
-      <c r="D506" t="s">
-        <v>942</v>
       </c>
       <c r="E506" t="s">
         <v>391</v>
@@ -12928,10 +12928,10 @@
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="B507" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C507" t="s">
         <v>522</v>
@@ -12945,10 +12945,10 @@
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="B508" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C508" t="s">
         <v>263</v>
@@ -12962,10 +12962,10 @@
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A509" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B509" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C509" t="s">
         <v>263</v>
@@ -12979,10 +12979,10 @@
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A510" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="B510" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="C510" t="s">
         <v>263</v>
@@ -12996,10 +12996,10 @@
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A511" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B511" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="C511" t="s">
         <v>398</v>
@@ -13013,13 +13013,13 @@
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="B512" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="C512" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="D512" t="s">
         <v>477</v>
@@ -13030,10 +13030,10 @@
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="B513" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="C513" t="s">
         <v>715</v>
@@ -13047,10 +13047,10 @@
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B514" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="C514" t="s">
         <v>263</v>
@@ -13064,10 +13064,10 @@
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B515" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="C515" t="s">
         <v>263</v>
@@ -13081,10 +13081,10 @@
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A516" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B516" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C516" t="s">
         <v>235</v>
@@ -13098,10 +13098,10 @@
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B517" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C517" t="s">
         <v>275</v>
@@ -13115,13 +13115,13 @@
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A518" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B518" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="C518" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D518" t="s">
         <v>530</v>
@@ -13132,10 +13132,10 @@
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="B519" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="C519" t="s">
         <v>266</v>
@@ -13144,15 +13144,15 @@
         <v>442</v>
       </c>
       <c r="E519" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A520" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B520" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="C520" t="s">
         <v>389</v>
@@ -13169,13 +13169,13 @@
         <v>198</v>
       </c>
       <c r="B521" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C521" t="s">
         <v>285</v>
       </c>
       <c r="D521" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="E521" t="s">
         <v>682</v>
@@ -13183,10 +13183,10 @@
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B522" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="C522" t="s">
         <v>340</v>
@@ -13200,13 +13200,13 @@
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
+        <v>965</v>
+      </c>
+      <c r="B523" t="s">
+        <v>966</v>
+      </c>
+      <c r="C523" t="s">
         <v>967</v>
-      </c>
-      <c r="B523" t="s">
-        <v>968</v>
-      </c>
-      <c r="C523" t="s">
-        <v>969</v>
       </c>
       <c r="D523" t="s">
         <v>271</v>
@@ -13217,10 +13217,10 @@
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="B524" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C524" t="s">
         <v>263</v>
@@ -13234,10 +13234,10 @@
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="B525" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="C525" t="s">
         <v>450</v>
@@ -13251,10 +13251,10 @@
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A526" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B526" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C526" t="s">
         <v>263</v>
@@ -13268,10 +13268,10 @@
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="B527" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="C527" t="s">
         <v>263</v>
@@ -13285,13 +13285,13 @@
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A528" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="B528" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="C528" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="D528" t="s">
         <v>471</v>
@@ -13302,10 +13302,10 @@
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="B529" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="C529" t="s">
         <v>715</v>
@@ -13322,7 +13322,7 @@
         <v>202</v>
       </c>
       <c r="B530" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="C530" t="s">
         <v>263</v>
@@ -13336,13 +13336,13 @@
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B531" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="C531" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D531" t="s">
         <v>282</v>
@@ -13353,16 +13353,16 @@
     </row>
     <row r="532" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="B532" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C532" t="s">
         <v>490</v>
       </c>
       <c r="D532" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="E532" t="s">
         <v>511</v>
@@ -13370,10 +13370,10 @@
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B533" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="C533" t="s">
         <v>473</v>
@@ -13387,10 +13387,10 @@
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="B534" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="C534" t="s">
         <v>674</v>
@@ -13404,10 +13404,10 @@
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="B535" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="C535" t="s">
         <v>425</v>
@@ -13421,13 +13421,13 @@
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="B536" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="C536" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D536" t="s">
         <v>275</v>
@@ -13438,16 +13438,16 @@
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="B537" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="C537" t="s">
         <v>442</v>
       </c>
       <c r="D537" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="E537" t="s">
         <v>463</v>
@@ -13455,10 +13455,10 @@
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B538" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="C538" t="s">
         <v>396</v>
@@ -13472,10 +13472,10 @@
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B539" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="C539" t="s">
         <v>263</v>
@@ -13489,10 +13489,10 @@
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B540" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="C540" t="s">
         <v>320</v>
@@ -13506,10 +13506,10 @@
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B541" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="C541" t="s">
         <v>244</v>
@@ -13523,10 +13523,10 @@
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B542" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="C542" t="s">
         <v>263</v>
@@ -13540,10 +13540,10 @@
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="B543" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="C543" t="s">
         <v>263</v>
@@ -13557,10 +13557,10 @@
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="B544" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="C544" t="s">
         <v>546</v>
@@ -13574,10 +13574,10 @@
     </row>
     <row r="545" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="B545" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C545" t="s">
         <v>434</v>
@@ -13591,10 +13591,10 @@
     </row>
     <row r="546" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B546" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="C546" t="s">
         <v>258</v>
@@ -13608,27 +13608,27 @@
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B547" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C547" t="s">
         <v>1003</v>
       </c>
-      <c r="B547" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C547" t="s">
-        <v>1005</v>
-      </c>
       <c r="D547" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="E547" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="B548" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="C548" t="s">
         <v>263</v>
@@ -13642,10 +13642,10 @@
     </row>
     <row r="549" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A549" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="B549" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="C549" t="s">
         <v>379</v>
@@ -13659,10 +13659,10 @@
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="B550" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="C550" t="s">
         <v>425</v>
@@ -13676,10 +13676,10 @@
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A551" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="B551" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="C551" t="s">
         <v>263</v>
@@ -13693,10 +13693,10 @@
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B552" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="C552" t="s">
         <v>268</v>
@@ -13710,10 +13710,10 @@
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A553" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B553" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="C553" t="s">
         <v>263</v>
@@ -13727,10 +13727,10 @@
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B554" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="C554" t="s">
         <v>375</v>
@@ -13744,10 +13744,10 @@
     </row>
     <row r="555" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A555" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="B555" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="C555" t="s">
         <v>263</v>
@@ -13761,10 +13761,10 @@
     </row>
     <row r="556" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="B556" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C556" t="s">
         <v>332</v>
@@ -13778,10 +13778,10 @@
     </row>
     <row r="557" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A557" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="B557" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="C557" t="s">
         <v>263</v>
@@ -13795,10 +13795,10 @@
     </row>
     <row r="558" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A558" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="B558" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="C558" t="s">
         <v>263</v>
@@ -13812,10 +13812,10 @@
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A559" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="B559" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="C559" t="s">
         <v>243</v>
@@ -13829,10 +13829,10 @@
     </row>
     <row r="560" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A560" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="B560" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="C560" t="s">
         <v>263</v>
@@ -13846,13 +13846,13 @@
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B561" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C561" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D561" t="s">
         <v>399</v>
@@ -13863,10 +13863,10 @@
     </row>
     <row r="562" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B562" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="C562" t="s">
         <v>263</v>
@@ -13880,10 +13880,10 @@
     </row>
     <row r="563" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="B563" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C563" t="s">
         <v>263</v>
@@ -13897,10 +13897,10 @@
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="B564" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C564" t="s">
         <v>343</v>
@@ -13914,10 +13914,10 @@
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="B565" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C565" t="s">
         <v>263</v>
@@ -13931,16 +13931,16 @@
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A566" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="B566" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C566" t="s">
         <v>340</v>
       </c>
       <c r="D566" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E566" t="s">
         <v>326</v>
@@ -13948,7 +13948,7 @@
     </row>
     <row r="567" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B567" t="s">
         <v>233</v>
@@ -13965,10 +13965,10 @@
     </row>
     <row r="568" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A568" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="B568" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="C568" t="s">
         <v>263</v>
@@ -13982,10 +13982,10 @@
     </row>
     <row r="569" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="B569" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C569" t="s">
         <v>263</v>
@@ -13999,13 +13999,13 @@
     </row>
     <row r="570" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B570" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C570" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="D570" t="s">
         <v>437</v>
@@ -14016,10 +14016,10 @@
     </row>
     <row r="571" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="B571" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="C571" t="s">
         <v>396</v>
@@ -14033,10 +14033,10 @@
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="B572" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C572" t="s">
         <v>378</v>
@@ -14050,10 +14050,10 @@
     </row>
     <row r="573" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="B573" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="C573" t="s">
         <v>307</v>
@@ -14067,10 +14067,10 @@
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="B574" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="C574" t="s">
         <v>250</v>
@@ -14084,10 +14084,10 @@
     </row>
     <row r="575" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="B575" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C575" t="s">
         <v>724</v>
@@ -14101,10 +14101,10 @@
     </row>
     <row r="576" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B576" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="C576" t="s">
         <v>461</v>
@@ -14118,10 +14118,10 @@
     </row>
     <row r="577" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="B577" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="C577" t="s">
         <v>263</v>
@@ -14135,10 +14135,10 @@
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="B578" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="C578" t="s">
         <v>263</v>
@@ -14152,10 +14152,10 @@
     </row>
     <row r="579" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="B579" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="C579" t="s">
         <v>263</v>
@@ -14169,10 +14169,10 @@
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A580" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="B580" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="C580" t="s">
         <v>349</v>
@@ -14186,10 +14186,10 @@
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A581" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="B581" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C581" t="s">
         <v>263</v>
@@ -14203,10 +14203,10 @@
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A582" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="B582" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="C582" t="s">
         <v>263</v>
@@ -14220,10 +14220,10 @@
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A583" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="B583" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="C583" t="s">
         <v>305</v>
@@ -14237,10 +14237,10 @@
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A584" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="B584" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="C584" t="s">
         <v>306</v>
@@ -14254,10 +14254,10 @@
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A585" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="B585" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="C585" t="s">
         <v>363</v>
@@ -14271,10 +14271,10 @@
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A586" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="B586" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="C586" t="s">
         <v>263</v>
@@ -14288,10 +14288,10 @@
     </row>
     <row r="587" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="B587" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="C587" t="s">
         <v>263</v>
@@ -14305,10 +14305,10 @@
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A588" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="B588" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="C588" t="s">
         <v>341</v>
@@ -14322,10 +14322,10 @@
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A589" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="B589" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="C589" t="s">
         <v>263</v>
@@ -14339,10 +14339,10 @@
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A590" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="B590" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C590" t="s">
         <v>263</v>
@@ -14356,10 +14356,10 @@
     </row>
     <row r="591" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A591" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="B591" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="C591" t="s">
         <v>263</v>
@@ -14373,10 +14373,10 @@
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A592" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="B592" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="C592" t="s">
         <v>263</v>
@@ -14390,10 +14390,10 @@
     </row>
     <row r="593" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="B593" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="C593" t="s">
         <v>263</v>
@@ -14407,10 +14407,10 @@
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A594" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="B594" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="C594" t="s">
         <v>263</v>
@@ -14424,10 +14424,10 @@
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="B595" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="C595" t="s">
         <v>557</v>
@@ -14441,10 +14441,10 @@
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A596" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="B596" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="C596" t="s">
         <v>525</v>
@@ -14458,10 +14458,10 @@
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A597" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="B597" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C597" t="s">
         <v>340</v>
@@ -14475,10 +14475,10 @@
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A598" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="B598" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="C598" t="s">
         <v>244</v>
@@ -14492,13 +14492,13 @@
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="B599" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="C599" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D599" t="s">
         <v>271</v>
@@ -14509,10 +14509,10 @@
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A600" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="B600" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="C600" t="s">
         <v>275</v>
@@ -14526,10 +14526,10 @@
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="B601" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="C601" t="s">
         <v>508</v>
@@ -14543,10 +14543,10 @@
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A602" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="B602" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="C602" t="s">
         <v>253</v>
@@ -14560,10 +14560,10 @@
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="B603" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="C603" t="s">
         <v>263</v>
@@ -14577,10 +14577,10 @@
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A604" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="B604" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="C604" t="s">
         <v>235</v>
@@ -14594,16 +14594,16 @@
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="B605" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="C605" t="s">
         <v>724</v>
       </c>
       <c r="D605" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="E605" t="s">
         <v>422</v>
@@ -14611,10 +14611,10 @@
     </row>
     <row r="606" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="B606" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="C606" t="s">
         <v>263</v>
@@ -14628,16 +14628,16 @@
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A607" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="B607" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C607" t="s">
         <v>331</v>
       </c>
       <c r="D607" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E607" t="s">
         <v>471</v>
@@ -14645,10 +14645,10 @@
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A608" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="B608" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="C608" t="s">
         <v>263</v>
@@ -14662,16 +14662,16 @@
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A609" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="B609" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="C609" t="s">
         <v>340</v>
       </c>
       <c r="D609" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="E609" t="s">
         <v>375</v>
@@ -14679,10 +14679,10 @@
     </row>
     <row r="610" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A610" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="B610" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="C610" t="s">
         <v>263</v>
@@ -14696,10 +14696,10 @@
     </row>
     <row r="611" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A611" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="B611" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="C611" t="s">
         <v>477</v>
@@ -14708,15 +14708,15 @@
         <v>277</v>
       </c>
       <c r="E611" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="612" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A612" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="B612" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="C612" t="s">
         <v>241</v>
@@ -14730,10 +14730,10 @@
     </row>
     <row r="613" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A613" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="B613" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="C613" t="s">
         <v>297</v>

</xml_diff>